<commit_message>
completed Array, ArrayTryEditor, Graph and GraphTryEditor done
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telan\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telan\git\dsAlgoBDDSigma\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DSAlgoLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="DSAlogRegister" sheetId="2" r:id="rId2"/>
+    <sheet name="ArrayTryEditor" sheetId="3" r:id="rId3"/>
+    <sheet name="GraphTryEditor" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -51,13 +54,101 @@
   </si>
   <si>
     <t>greenHorn@2024</t>
+  </si>
+  <si>
+    <t>arraySubPage</t>
+  </si>
+  <si>
+    <t>testCase</t>
+  </si>
+  <si>
+    <t>actions</t>
+  </si>
+  <si>
+    <t>expectedResults</t>
+  </si>
+  <si>
+    <t>withoutCodeRun</t>
+  </si>
+  <si>
+    <t>with empty window</t>
+  </si>
+  <si>
+    <t>invalidCodeRun</t>
+  </si>
+  <si>
+    <t>with invalid code</t>
+  </si>
+  <si>
+    <t>validCodeRun</t>
+  </si>
+  <si>
+    <t>with valid code</t>
+  </si>
+  <si>
+    <t>Arrays Using List</t>
+  </si>
+  <si>
+    <t>Basic Operations In Lists</t>
+  </si>
+  <si>
+    <t>Applications Of Array</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>NameError</t>
+  </si>
+  <si>
+    <t>sprint("HelloWorld)</t>
+  </si>
+  <si>
+    <t>print("Hello, World!")</t>
+  </si>
+  <si>
+    <t>Output displayed in the console</t>
+  </si>
+  <si>
+    <t>SyntaxError</t>
+  </si>
+  <si>
+    <t>arrays in python</t>
+  </si>
+  <si>
+    <t>Defect</t>
+  </si>
+  <si>
+    <t>graphSubPage</t>
+  </si>
+  <si>
+    <t># Print numbers from 1 to 10
+for i in range(1, 11):
+  print(i)</t>
+  </si>
+  <si>
+    <t># Print numbers from 1 to 10
+for i in range(1, 11:
+  print(i)</t>
+  </si>
+  <si>
+    <t>pythoncde</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>graph representations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +163,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,9 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,4 +555,487 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Graph, GraphTryEditor and ArrayPracticeQns
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DSAlgoLogin" sheetId="1" r:id="rId1"/>
     <sheet name="DSAlogRegister" sheetId="2" r:id="rId2"/>
     <sheet name="ArrayTryEditor" sheetId="3" r:id="rId3"/>
     <sheet name="GraphTryEditor" sheetId="4" r:id="rId4"/>
+    <sheet name="ArrayPracticeQns" sheetId="5" r:id="rId5"/>
+    <sheet name="Defects" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="80">
   <si>
     <t>username</t>
   </si>
@@ -142,13 +144,184 @@
   </si>
   <si>
     <t>graph representations</t>
+  </si>
+  <si>
+    <t>ExistingCodeSnippet</t>
+  </si>
+  <si>
+    <t>InvalidCodeSnippet</t>
+  </si>
+  <si>
+    <t>VaildCodeSnippet</t>
+  </si>
+  <si>
+    <t>errRun</t>
+  </si>
+  <si>
+    <t>errSubmit</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>def (input_list, num):
+    if num in input_list:
+        print("Element Found")
+    else:
+        print("Not Found)</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+    if num in input_list:
+        print("Element Found")
+    else:
+        print("Not Found")
+# Example usage
+search([12, 23, 45, 67, 6, 90], 12)  # Output: Element Found
+search([12, 23, 45, 67, 6, 90], 25)  # Output: Not Found</t>
+  </si>
+  <si>
+    <t>questions</t>
+  </si>
+  <si>
+    <t>OutputDisplayed</t>
+  </si>
+  <si>
+    <t>search the array</t>
+  </si>
+  <si>
+    <t>max consecutive ones</t>
+  </si>
+  <si>
+    <t>find numbers with even number of digits</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findMaxConsecutiveOnes(nums) :
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0
+    return max_count
+print(findMaxConsecutiveOnes([1, 1, 0, 1, 1, 1]))  # Output: 3
+print(findMaxConsecutiveOnes([1, 0, 1, 1, 0, 1]))  # Output: 2
+</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> findMaxConsecutiveOnes(nums) :
+    max_count = 0
+    current_count = 0</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+# Example usage
+print(findNumbers([12, 345, 2, 6, 7896]))   # Output: 2
+print(findNumbers([555, 901, 482, 1771]))   # Output: 1
+</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums)
+    count = 0</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+    return sorted([x * x for x in nums])
+# Example usage
+print(sortedSquares([-4, -1, 0, 3, 10]))  # Output: [0, 1, 9, 16, 100]
+print(sortedSquares([-7, -3, 2, 3, 11]))  # Output: [4, 9, 9, 49, 121]
+</t>
+  </si>
+  <si>
+    <t>codeValidations</t>
+  </si>
+  <si>
+    <t>squares of  a sorted array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+    return sorted([x * x for x in nums]
+</t>
+  </si>
+  <si>
+    <t>EmptyRun</t>
+  </si>
+  <si>
+    <t>InvalidCodeRun</t>
+  </si>
+  <si>
+    <t>ValidCodeRun</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>FeatureName</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Defect/Not</t>
+  </si>
+  <si>
+    <t>ScreenShot(Y/N)</t>
+  </si>
+  <si>
+    <t>RaiseBugJira(Y/N)</t>
+  </si>
+  <si>
+    <t>ArrayTryEditor</t>
+  </si>
+  <si>
+    <t>DisplayAlert</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>PageName</t>
+  </si>
+  <si>
+    <t>GraphTryEditor</t>
+  </si>
+  <si>
+    <t>QnsDisplayedInPraticePage</t>
+  </si>
+  <si>
+    <t>DisplayQuestions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +342,13 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,13 +371,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +663,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +758,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A17" activeCellId="3" sqref="A5 A9 A13 A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,170 +1054,598 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E9" t="s">
-        <v>27</v>
+      <c r="D9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed Login, updated hooks for afterSignIn and updated excelreader
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DSAlgoLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="DSAlogRegister" sheetId="2" r:id="rId2"/>
-    <sheet name="ArrayTryEditor" sheetId="3" r:id="rId3"/>
-    <sheet name="GraphTryEditor" sheetId="4" r:id="rId4"/>
-    <sheet name="ArrayPracticeQns" sheetId="5" r:id="rId5"/>
-    <sheet name="Defects" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="DSAlogRegister" sheetId="2" r:id="rId3"/>
+    <sheet name="ArrayTryEditor" sheetId="3" r:id="rId4"/>
+    <sheet name="GraphTryEditor" sheetId="4" r:id="rId5"/>
+    <sheet name="ArrayPracticeQns" sheetId="5" r:id="rId6"/>
+    <sheet name="Defects" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="82">
   <si>
     <t>username</t>
   </si>
@@ -37,9 +38,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>messages</t>
-  </si>
-  <si>
     <t>asxcvb</t>
   </si>
   <si>
@@ -52,9 +50,6 @@
     <t>numpyninja</t>
   </si>
   <si>
-    <t>Invalid username and password</t>
-  </si>
-  <si>
     <t>greenHorn@2024</t>
   </si>
   <si>
@@ -64,30 +59,12 @@
     <t>testCase</t>
   </si>
   <si>
-    <t>actions</t>
-  </si>
-  <si>
     <t>expectedResults</t>
   </si>
   <si>
     <t>withoutCodeRun</t>
   </si>
   <si>
-    <t>with empty window</t>
-  </si>
-  <si>
-    <t>invalidCodeRun</t>
-  </si>
-  <si>
-    <t>with invalid code</t>
-  </si>
-  <si>
-    <t>validCodeRun</t>
-  </si>
-  <si>
-    <t>with valid code</t>
-  </si>
-  <si>
     <t>Arrays Using List</t>
   </si>
   <si>
@@ -103,16 +80,10 @@
     <t>NumpyNinja</t>
   </si>
   <si>
-    <t>NameError</t>
-  </si>
-  <si>
     <t>sprint("HelloWorld)</t>
   </si>
   <si>
     <t>print("Hello, World!")</t>
-  </si>
-  <si>
-    <t>Output displayed in the console</t>
   </si>
   <si>
     <t>SyntaxError</t>
@@ -324,6 +295,33 @@
   </si>
   <si>
     <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>ValidCredential</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t>EmptyPwd</t>
+  </si>
+  <si>
+    <t>EmptyUserName</t>
+  </si>
+  <si>
+    <t>WrongUserName</t>
+  </si>
+  <si>
+    <t>WrongPwd</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
   </si>
 </sst>
 </file>
@@ -678,77 +676,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -758,6 +775,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -771,297 +800,245 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" activeCellId="3" sqref="A5 A9 A13 A17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
       <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
       <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
       <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
       <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1070,12 +1047,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,122 +1065,122 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1212,12 +1189,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,224 +1208,224 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1457,12 +1434,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,7 +1448,7 @@
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -1479,268 +1456,268 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed Stack, Queue, LInkedlist
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telan\git\dsAlgoBDDSigma\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSAlgoBDD\DSAlgoBDDGit\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2668481-20B8-4368-9514-8CB731CE8BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8484" windowHeight="5268" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSAlgoLogin" sheetId="1" r:id="rId1"/>
@@ -18,6 +19,9 @@
     <sheet name="GraphTryEditor" sheetId="4" r:id="rId4"/>
     <sheet name="ArrayPracticeQns" sheetId="5" r:id="rId5"/>
     <sheet name="Defects" sheetId="6" r:id="rId6"/>
+    <sheet name="LinkedListTryEditor" sheetId="8" r:id="rId7"/>
+    <sheet name="QueueTryEditor" sheetId="9" r:id="rId8"/>
+    <sheet name="StackTryEditor" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="104">
   <si>
     <t>username</t>
   </si>
@@ -325,12 +329,75 @@
   <si>
     <t>No tests were collected</t>
   </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applications </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traversal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insertion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deletion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmptyRun </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> InvalidCodeRun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OutputDisplayed </t>
+  </si>
+  <si>
+    <t>Implementation of Queue in python</t>
+  </si>
+  <si>
+    <t>Implementation using array</t>
+  </si>
+  <si>
+    <t>Implementation using collections.deque</t>
+  </si>
+  <si>
+    <t>Queue Operations</t>
+  </si>
+  <si>
+    <t>queueSubPage</t>
+  </si>
+  <si>
+    <t>stackSubPage</t>
+  </si>
+  <si>
+    <t>Operations in Stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction </t>
+  </si>
+  <si>
+    <t>Creating Linked LIst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types of Linked List </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Linked List in Python </t>
+  </si>
+  <si>
+    <t xml:space="preserve">linkedListSubPage </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +432,12 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -386,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,10 +467,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,21 +755,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -710,7 +788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -718,7 +796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -729,7 +807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -740,7 +818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -758,28 +836,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" activeCellId="3" sqref="A5 A9 A13 A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
@@ -787,7 +865,7 @@
     <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -804,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -818,7 +896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -835,7 +913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -852,7 +930,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -869,7 +947,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -883,7 +961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -900,7 +978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -917,7 +995,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -934,7 +1012,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -948,7 +1026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -965,7 +1043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -982,7 +1060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -999,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1013,7 +1091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1108,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1047,7 +1125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1071,14 +1149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
@@ -1086,7 +1164,7 @@
     <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1100,7 +1178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1111,7 +1189,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1125,7 +1203,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="57.6">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -1139,7 +1217,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="57.6">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
@@ -1153,7 +1231,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1164,7 +1242,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1178,7 +1256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="57.6">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1192,7 +1270,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="57.6">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1213,14 +1291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
@@ -1229,7 +1307,7 @@
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1246,7 +1324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1263,7 +1341,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="72">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1280,7 +1358,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="158.4">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1297,7 +1375,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1314,7 +1392,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1331,7 +1409,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="259.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1348,7 +1426,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1365,7 +1443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1382,7 +1460,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="172.8">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1399,7 +1477,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1416,7 +1494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.2">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1426,15 +1504,14 @@
       <c r="C12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" ht="129.6">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1458,14 +1535,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -1477,7 +1554,7 @@
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -1503,7 +1580,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1523,7 +1600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1543,7 +1620,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1563,7 +1640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1583,7 +1660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1603,7 +1680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1616,14 +1693,14 @@
       <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -1636,14 +1713,14 @@
       <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -1663,7 +1740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -1683,7 +1760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1703,7 +1780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -1723,7 +1800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1747,4 +1824,900 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3DA11F-6B7C-4131-868B-DC2C94AE10B2}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304714D6-CBA6-4AA4-9E3F-8972FEDDE24F}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDF3BEC-0CDE-4AC9-BB23-A2911998F997}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="8"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="8"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="8"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="8"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Jenkins issue on testReRunner.FailedRun
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java_workspace\DSAlgoBDDGit\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telan\git\dsAlgoBDDSigma\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8CD603-CC7B-440A-8F78-788B301BFBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DSAlgoLogin" sheetId="1" r:id="rId1"/>
@@ -400,24 +399,12 @@
     <t>EmptyPassword</t>
   </si>
   <si>
-    <t>WrongPassword</t>
-  </si>
-  <si>
     <t>ShortPassword</t>
   </si>
   <si>
     <t>NumaricPassword</t>
   </si>
   <si>
-    <t>expectedmessage</t>
-  </si>
-  <si>
-    <t>pass12</t>
-  </si>
-  <si>
-    <t>password_mismatch</t>
-  </si>
-  <si>
     <t>qwer</t>
   </si>
   <si>
@@ -458,13 +445,25 @@
   </si>
   <si>
     <t>New Account Created</t>
+  </si>
+  <si>
+    <t>TreeTryEditor</t>
+  </si>
+  <si>
+    <t>MismatchPassword</t>
+  </si>
+  <si>
+    <t>pass23</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -531,12 +530,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,14 +829,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -831,7 +844,7 @@
     <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -842,10 +855,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -856,12 +869,12 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -870,12 +883,12 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -884,12 +897,12 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -898,9 +911,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -916,14 +929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" customWidth="1"/>
@@ -932,28 +945,28 @@
     <col min="5" max="5" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="E1" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="6"/>
+        <v>119</v>
+      </c>
+      <c r="B2" s="12"/>
       <c r="C2" s="6" t="s">
         <v>100</v>
       </c>
@@ -961,128 +974,129 @@
         <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="E5" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="B6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="11">
+        <v>123456</v>
+      </c>
+      <c r="D7" s="11">
+        <v>123456</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8">
-      <c r="A6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8">
-      <c r="A7" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="7">
-        <v>123456</v>
-      </c>
-      <c r="D7" s="7">
-        <v>123456</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>126</v>
+      <c r="E8" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1107,7 +1121,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1121,7 +1135,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1135,7 +1149,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1149,7 +1163,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1160,7 +1174,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1174,7 +1188,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1188,7 +1202,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1202,7 +1216,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1227,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1227,7 +1241,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1241,7 +1255,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1255,7 +1269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1266,7 +1280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1280,7 +1294,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1294,7 +1308,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1315,14 +1329,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
@@ -1330,7 +1344,7 @@
     <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1344,7 +1358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1355,7 +1369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.6">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="57.6">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1397,7 +1411,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1408,7 +1422,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1422,7 +1436,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57.6">
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1450,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.6">
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1457,14 +1471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
@@ -1473,7 +1487,7 @@
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1490,7 +1504,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1507,7 +1521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="158.4">
+    <row r="4" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1541,7 +1555,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1575,7 +1589,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="259.2">
+    <row r="7" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1592,7 +1606,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1609,7 +1623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1626,7 +1640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="172.8">
+    <row r="10" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1643,7 +1657,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1660,7 +1674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.2">
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="129.6">
+    <row r="13" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1701,14 +1715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.5546875" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -1716,7 +1730,7 @@
     <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -1730,7 +1744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1741,7 +1755,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1755,7 +1769,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1769,7 +1783,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1783,7 +1797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1794,7 +1808,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -1808,7 +1822,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -1822,7 +1836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1836,7 +1850,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1847,7 +1861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1861,7 +1875,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1875,7 +1889,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1889,7 +1903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1900,7 +1914,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1914,7 +1928,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -1928,7 +1942,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1942,7 +1956,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1953,7 +1967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1967,7 +1981,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -1981,7 +1995,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1995,7 +2009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -2006,7 +2020,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -2020,7 +2034,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2034,7 +2048,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -2048,7 +2062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -2059,7 +2073,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -2073,7 +2087,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -2087,7 +2101,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -2101,7 +2115,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -2112,7 +2126,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2126,7 +2140,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -2140,7 +2154,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -2154,7 +2168,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -2165,7 +2179,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -2179,7 +2193,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -2193,7 +2207,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2207,7 +2221,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2218,7 +2232,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2232,7 +2246,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2246,7 +2260,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2260,7 +2274,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2271,7 +2285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -2285,7 +2299,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2299,7 +2313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2313,7 +2327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2324,7 +2338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2338,7 +2352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -2352,7 +2366,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -2366,7 +2380,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -2377,7 +2391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -2391,7 +2405,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -2405,7 +2419,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>91</v>
       </c>
@@ -2426,14 +2440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
@@ -2445,7 +2459,7 @@
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2471,7 +2485,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2491,7 +2505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2511,7 +2525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2531,7 +2545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2551,7 +2565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -2571,7 +2585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2591,7 +2605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -2611,7 +2625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -2631,7 +2645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2651,7 +2665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2671,7 +2685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2691,7 +2705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2711,9 +2725,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
         <v>74</v>
@@ -2731,9 +2745,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
         <v>92</v>
@@ -2751,9 +2765,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
         <v>81</v>
@@ -2771,9 +2785,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
         <v>93</v>
@@ -2791,9 +2805,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
         <v>94</v>
@@ -2811,9 +2825,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>84</v>
@@ -2831,9 +2845,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
         <v>95</v>
@@ -2851,9 +2865,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
         <v>86</v>
@@ -2871,9 +2885,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
         <v>87</v>
@@ -2891,9 +2905,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
         <v>88</v>
@@ -2911,9 +2925,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -2931,9 +2945,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
@@ -2951,9 +2965,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B26" t="s">
         <v>91</v>
@@ -2971,9 +2985,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="B27" t="s">
         <v>74</v>
@@ -2991,9 +3005,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
@@ -3011,9 +3025,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
         <v>81</v>
@@ -3031,9 +3045,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
         <v>93</v>
@@ -3051,9 +3065,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
         <v>94</v>
@@ -3071,9 +3085,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
         <v>84</v>
@@ -3091,9 +3105,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
@@ -3111,9 +3125,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
         <v>89</v>
@@ -3131,9 +3145,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
         <v>90</v>
@@ -3151,9 +3165,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
         <v>91</v>
@@ -3171,9 +3185,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
         <v>95</v>
@@ -3191,9 +3205,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B38" t="s">
         <v>86</v>
@@ -3211,9 +3225,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
         <v>87</v>
@@ -3229,6 +3243,9 @@
       </c>
       <c r="F39" t="s">
         <v>20</v>
+      </c>
+      <c r="G39">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for cross browser and parallel testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="160">
   <si>
     <t>username</t>
   </si>
@@ -554,6 +554,12 @@
   </si>
   <si>
     <t>Getting password mismatch error message</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>Max ConsecutiveOnes</t>
   </si>
 </sst>
 </file>
@@ -1290,11 +1296,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1436,27 +1442,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>159</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>70</v>
       </c>
@@ -1464,19 +1470,19 @@
         <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="21" t="s">
         <v>72</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>70</v>
       </c>
@@ -1484,33 +1490,33 @@
         <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>20</v>
@@ -1521,7 +1527,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
@@ -1541,13 +1547,13 @@
         <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>65</v>
@@ -1561,7 +1567,7 @@
         <v>67</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>68</v>
@@ -1578,16 +1584,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>65</v>
@@ -1601,7 +1607,7 @@
         <v>123</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
@@ -1621,7 +1627,7 @@
         <v>123</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
@@ -1641,7 +1647,7 @@
         <v>123</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
@@ -1661,7 +1667,7 @@
         <v>123</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
@@ -1681,7 +1687,7 @@
         <v>123</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
@@ -1701,7 +1707,7 @@
         <v>123</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>10</v>
@@ -1721,7 +1727,7 @@
         <v>123</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
@@ -1741,7 +1747,7 @@
         <v>123</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
@@ -1761,7 +1767,7 @@
         <v>123</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
@@ -1781,7 +1787,7 @@
         <v>123</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
@@ -1801,7 +1807,7 @@
         <v>123</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>10</v>
@@ -1821,7 +1827,7 @@
         <v>123</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
@@ -1841,13 +1847,13 @@
         <v>123</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>65</v>
@@ -1861,7 +1867,7 @@
         <v>123</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>68</v>
@@ -1881,7 +1887,7 @@
         <v>123</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>68</v>
@@ -1901,7 +1907,7 @@
         <v>123</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>68</v>
@@ -1921,7 +1927,7 @@
         <v>123</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>68</v>
@@ -1941,7 +1947,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>68</v>
@@ -1961,7 +1967,7 @@
         <v>123</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>68</v>
@@ -1981,7 +1987,7 @@
         <v>123</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>68</v>
@@ -2001,7 +2007,7 @@
         <v>123</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>68</v>
@@ -2021,7 +2027,7 @@
         <v>123</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>68</v>
@@ -2041,7 +2047,7 @@
         <v>123</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>68</v>
@@ -2061,7 +2067,7 @@
         <v>123</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>68</v>
@@ -2081,7 +2087,7 @@
         <v>123</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>68</v>
@@ -2098,10 +2104,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>68</v>
@@ -2124,10 +2130,10 @@
         <v>146</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>65</v>
@@ -2138,16 +2144,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>65</v>
@@ -2161,7 +2167,7 @@
         <v>152</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>68</v>
@@ -2181,7 +2187,7 @@
         <v>152</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>68</v>
@@ -2201,13 +2207,13 @@
         <v>152</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>65</v>
@@ -2221,7 +2227,7 @@
         <v>152</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>10</v>
@@ -2241,7 +2247,7 @@
         <v>152</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>10</v>
@@ -2256,18 +2262,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>65</v>
@@ -2281,7 +2287,7 @@
         <v>153</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>68</v>
@@ -2296,12 +2302,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>68</v>
@@ -2321,7 +2327,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>68</v>
@@ -2336,18 +2342,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>65</v>
@@ -2361,7 +2367,7 @@
         <v>153</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>10</v>
@@ -2376,12 +2382,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>10</v>
@@ -2401,7 +2407,7 @@
         <v>153</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>10</v>
@@ -2418,16 +2424,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>65</v>
@@ -2441,7 +2447,7 @@
         <v>154</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>68</v>
@@ -2461,7 +2467,7 @@
         <v>154</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>68</v>
@@ -2481,7 +2487,7 @@
         <v>154</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>68</v>
@@ -2501,7 +2507,7 @@
         <v>154</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>68</v>
@@ -2521,7 +2527,7 @@
         <v>154</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>68</v>
@@ -2541,13 +2547,13 @@
         <v>154</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>65</v>
@@ -2561,7 +2567,7 @@
         <v>154</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>10</v>
@@ -2581,7 +2587,7 @@
         <v>154</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>10</v>
@@ -2601,7 +2607,7 @@
         <v>154</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>10</v>
@@ -2621,7 +2627,7 @@
         <v>154</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>10</v>
@@ -2641,7 +2647,7 @@
         <v>154</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>10</v>
@@ -2656,43 +2662,103 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="C71" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+      <c r="F71" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="C72" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F72" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3248,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>